<commit_message>
Update Normalização de Tabelas.xlsx
</commit_message>
<xml_diff>
--- a/Documents/Normalização de Tabelas.xlsx
+++ b/Documents/Normalização de Tabelas.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="61">
   <si>
     <t>Tabelas não normalizadas</t>
   </si>
@@ -182,6 +182,15 @@
   </si>
   <si>
     <t>Estrategia</t>
+  </si>
+  <si>
+    <t>Usuario_has_Jogo</t>
+  </si>
+  <si>
+    <t>ID_Usuario</t>
+  </si>
+  <si>
+    <t>ID_Jogo</t>
   </si>
   <si>
     <t>XBOX 360</t>
@@ -370,7 +379,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -474,6 +483,9 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="11" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -1109,12 +1121,16 @@
     </row>
     <row r="20">
       <c r="A20" s="1"/>
-      <c r="B20" s="12" t="s">
+      <c r="B20" s="39" t="s">
         <v>5</v>
       </c>
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
       <c r="E20" s="11"/>
+      <c r="G20" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="H20" s="10"/>
     </row>
     <row r="21">
       <c r="A21" s="1"/>
@@ -1130,6 +1146,12 @@
       <c r="E21" s="16" t="s">
         <v>14</v>
       </c>
+      <c r="G21" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="H21" s="13" t="s">
+        <v>59</v>
+      </c>
       <c r="P21" s="1"/>
     </row>
     <row r="22">
@@ -1146,6 +1168,12 @@
       <c r="E22" s="22">
         <v>1.0425E8</v>
       </c>
+      <c r="G22" s="17">
+        <v>123457.0</v>
+      </c>
+      <c r="H22" s="17">
+        <v>346312.0</v>
+      </c>
       <c r="P22" s="1"/>
       <c r="Q22" s="1"/>
     </row>
@@ -1163,6 +1191,12 @@
       <c r="E23" s="22">
         <v>1.5768E8</v>
       </c>
+      <c r="G23" s="17">
+        <v>131000.0</v>
+      </c>
+      <c r="H23" s="17">
+        <v>513242.0</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="1"/>
@@ -1178,6 +1212,12 @@
       <c r="E24" s="22">
         <v>8.691E7</v>
       </c>
+      <c r="G24" s="17">
+        <v>253531.0</v>
+      </c>
+      <c r="H24" s="17">
+        <v>613589.0</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="1"/>
@@ -1193,6 +1233,12 @@
       <c r="E25" s="22">
         <v>8.806E7</v>
       </c>
+      <c r="G25" s="17">
+        <v>98190.0</v>
+      </c>
+      <c r="H25" s="17">
+        <v>434573.0</v>
+      </c>
       <c r="P25" s="1"/>
     </row>
     <row r="26">
@@ -1201,7 +1247,7 @@
         <v>101451.0</v>
       </c>
       <c r="C26" s="18" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D26" s="18" t="s">
         <v>24</v>

</xml_diff>